<commit_message>
This is my Second Commit Test Data changed
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\DataDrivenFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_2020\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61481FB-350A-43C9-8B66-2EF0BACAF258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -37,9 +38,6 @@
     <t>postcode</t>
   </si>
   <si>
-    <t>Raman</t>
-  </si>
-  <si>
     <t>Arora</t>
   </si>
   <si>
@@ -58,21 +56,9 @@
     <t>currency</t>
   </si>
   <si>
-    <t>Raman Arora</t>
-  </si>
-  <si>
     <t>Rupee</t>
   </si>
   <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Ishita</t>
-  </si>
-  <si>
-    <t>Rohit</t>
-  </si>
-  <si>
     <t>Sehgal</t>
   </si>
   <si>
@@ -98,12 +84,27 @@
   </si>
   <si>
     <t>runmode</t>
+  </si>
+  <si>
+    <t>Haresh</t>
+  </si>
+  <si>
+    <t>Deepak</t>
+  </si>
+  <si>
+    <t>Ashfaq</t>
+  </si>
+  <si>
+    <t>Atul</t>
+  </si>
+  <si>
+    <t>Haresh Vaity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,7 +415,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -425,34 +426,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -461,11 +462,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,78 +482,78 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -561,29 +562,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>